<commit_message>
Primera parte de la implementación del caso de uso pago alumno
Se implementa la primera parte del modulo registrar pago de alumno y consultar pagos de alumnos.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 4ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 4ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62247E5F-7292-47DF-82C1-67B1F3595668}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{94C6F61A-8B34-49C2-A786-78B85E623C08}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -484,8 +484,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{50A9524B-2953-46BD-B5A3-393E862A4C34}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1091,104 +1119,102 @@
       <c r="G6" s="5">
         <v>1</v>
       </c>
-      <c r="H6" s="8">
-        <v>1</v>
-      </c>
+      <c r="H6" s="8"/>
       <c r="I6" s="8">
         <f>G6-H6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8">
         <f t="shared" ref="L6:L17" si="0">I6-K6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8">
         <f t="shared" ref="O6:O17" si="1">L6-N6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8">
         <f t="shared" ref="R6:R17" si="2">O6-Q6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6" s="10"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8">
         <f t="shared" ref="U6:U17" si="3">R6-T6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8">
         <f t="shared" ref="X6:X17" si="4">U6-W6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y6" s="10"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8">
         <f t="shared" ref="AA6:AA17" si="5">X6-Z6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB6" s="10"/>
       <c r="AC6" s="8"/>
       <c r="AD6" s="8">
         <f t="shared" ref="AD6:AD17" si="6">AA6-AC6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE6" s="10"/>
       <c r="AF6" s="8"/>
       <c r="AG6" s="8">
         <f t="shared" ref="AG6:AG17" si="7">AD6-AF6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH6" s="10"/>
       <c r="AI6" s="8"/>
       <c r="AJ6" s="8">
         <f t="shared" ref="AJ6:AJ17" si="8">AG6-AI6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK6" s="10"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8">
         <f t="shared" ref="AM6:AM17" si="9">AJ6-AL6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN6" s="10"/>
       <c r="AO6" s="8"/>
       <c r="AP6" s="8">
         <f t="shared" ref="AP6:AP17" si="10">AM6-AO6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ6" s="10"/>
       <c r="AR6" s="8"/>
       <c r="AS6" s="8">
         <f t="shared" ref="AS6:AS17" si="11">AP6-AR6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT6" s="10"/>
       <c r="AU6" s="8"/>
       <c r="AV6" s="8">
         <f t="shared" ref="AV6:AV17" si="12">AS6-AU6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW6" s="10"/>
       <c r="AX6" s="8"/>
       <c r="AY6" s="8">
         <f t="shared" ref="AY6:AY17" si="13">AV6-AX6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ6" s="11">
         <f t="shared" ref="AZ6:AZ17" si="14">H6+K6+N6+Q6+T6+W6+Z6+AC6+AF6+AI6+AL6+AO6+AR6+AU6+AX6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA6" s="11">
         <f t="shared" ref="BA6:BA17" si="15">G6-AZ6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:53" ht="120" x14ac:dyDescent="0.25">
@@ -1206,102 +1232,104 @@
       <c r="G7" s="5">
         <v>4</v>
       </c>
-      <c r="H7" s="8"/>
+      <c r="H7" s="8">
+        <v>2</v>
+      </c>
       <c r="I7" s="8">
         <f t="shared" ref="I7:I17" si="16">G7-H7</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S7" s="10"/>
       <c r="T7" s="8"/>
       <c r="U7" s="8">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="8"/>
       <c r="X7" s="8">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y7" s="10"/>
       <c r="Z7" s="8"/>
       <c r="AA7" s="8">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB7" s="10"/>
       <c r="AC7" s="8"/>
       <c r="AD7" s="8">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE7" s="10"/>
       <c r="AF7" s="8"/>
       <c r="AG7" s="8">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AH7" s="10"/>
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AK7" s="10"/>
       <c r="AL7" s="8"/>
       <c r="AM7" s="8">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AN7" s="10"/>
       <c r="AO7" s="8"/>
       <c r="AP7" s="8">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AQ7" s="10"/>
       <c r="AR7" s="8"/>
       <c r="AS7" s="8">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AT7" s="10"/>
       <c r="AU7" s="8"/>
       <c r="AV7" s="8">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AW7" s="10"/>
       <c r="AX7" s="8"/>
       <c r="AY7" s="8">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AZ7" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA7" s="11">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:53" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modulo de pagos CRUPromocion e historial de pago de alumnos
Se implementa el caso e uso CRUPromocion, la consulta de promociones de
un alumno, registro de pagos de alumno asi como el historial de pagos de
alumno
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 4ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 4ta Iteración.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
-  <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDA813B-3555-4C93-8673-53DF2B8E2394}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -216,7 +210,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -484,8 +478,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -783,14 +805,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA20"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Z10" sqref="Z10"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,66 +1274,68 @@
         <v>-9</v>
       </c>
       <c r="Y7" s="10"/>
-      <c r="Z7" s="8"/>
+      <c r="Z7" s="8">
+        <v>6</v>
+      </c>
       <c r="AA7" s="8">
         <f t="shared" si="5"/>
-        <v>-9</v>
+        <v>-15</v>
       </c>
       <c r="AB7" s="10"/>
       <c r="AC7" s="8"/>
       <c r="AD7" s="8">
         <f t="shared" si="6"/>
-        <v>-9</v>
+        <v>-15</v>
       </c>
       <c r="AE7" s="10"/>
       <c r="AF7" s="8"/>
       <c r="AG7" s="8">
         <f t="shared" si="7"/>
-        <v>-9</v>
+        <v>-15</v>
       </c>
       <c r="AH7" s="10"/>
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8">
         <f t="shared" si="8"/>
-        <v>-9</v>
+        <v>-15</v>
       </c>
       <c r="AK7" s="10"/>
       <c r="AL7" s="8"/>
       <c r="AM7" s="8">
         <f t="shared" si="9"/>
-        <v>-9</v>
+        <v>-15</v>
       </c>
       <c r="AN7" s="10"/>
       <c r="AO7" s="8"/>
       <c r="AP7" s="8">
         <f t="shared" si="10"/>
-        <v>-9</v>
+        <v>-15</v>
       </c>
       <c r="AQ7" s="10"/>
       <c r="AR7" s="8"/>
       <c r="AS7" s="8">
         <f t="shared" si="11"/>
-        <v>-9</v>
+        <v>-15</v>
       </c>
       <c r="AT7" s="10"/>
       <c r="AU7" s="8"/>
       <c r="AV7" s="8">
         <f t="shared" si="12"/>
-        <v>-9</v>
+        <v>-15</v>
       </c>
       <c r="AW7" s="10"/>
       <c r="AX7" s="8"/>
       <c r="AY7" s="8">
         <f t="shared" si="13"/>
-        <v>-9</v>
+        <v>-15</v>
       </c>
       <c r="AZ7" s="11">
         <f t="shared" si="14"/>
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="BA7" s="11">
         <f t="shared" si="15"/>
-        <v>-9</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="8" spans="2:53" ht="45" x14ac:dyDescent="0.25">
@@ -2788,6 +2812,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2799,11 +2828,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2821,7 +2845,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Se termina el modulo de pagos
Se termina y corrigen partes del modulo de pagos e integracion del registro de pagos.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 4ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 4ta Iteración.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0BFF09B2-0032-4042-9D56-D593BBCAD538}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -210,7 +216,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -503,7 +509,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -562,7 +568,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -595,9 +601,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -630,6 +653,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -805,14 +845,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BA20"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,60 +1322,62 @@
         <v>-15</v>
       </c>
       <c r="AB7" s="10"/>
-      <c r="AC7" s="8"/>
+      <c r="AC7" s="8">
+        <v>1</v>
+      </c>
       <c r="AD7" s="8">
         <f t="shared" si="6"/>
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="AE7" s="10"/>
       <c r="AF7" s="8"/>
       <c r="AG7" s="8">
         <f t="shared" si="7"/>
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="AH7" s="10"/>
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8">
         <f t="shared" si="8"/>
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="AK7" s="10"/>
       <c r="AL7" s="8"/>
       <c r="AM7" s="8">
         <f t="shared" si="9"/>
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="AN7" s="10"/>
       <c r="AO7" s="8"/>
       <c r="AP7" s="8">
         <f t="shared" si="10"/>
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="AQ7" s="10"/>
       <c r="AR7" s="8"/>
       <c r="AS7" s="8">
         <f t="shared" si="11"/>
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="AT7" s="10"/>
       <c r="AU7" s="8"/>
       <c r="AV7" s="8">
         <f t="shared" si="12"/>
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="AW7" s="10"/>
       <c r="AX7" s="8"/>
       <c r="AY7" s="8">
         <f t="shared" si="13"/>
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="AZ7" s="11">
         <f t="shared" si="14"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="BA7" s="11">
         <f t="shared" si="15"/>
-        <v>-15</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="8" spans="2:53" ht="45" x14ac:dyDescent="0.25">
@@ -1395,60 +1437,62 @@
         <v>2</v>
       </c>
       <c r="AB8" s="10"/>
-      <c r="AC8" s="8"/>
+      <c r="AC8" s="8">
+        <v>1</v>
+      </c>
       <c r="AD8" s="8">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE8" s="10"/>
       <c r="AF8" s="8"/>
       <c r="AG8" s="8">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH8" s="10"/>
       <c r="AI8" s="8"/>
       <c r="AJ8" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK8" s="10"/>
       <c r="AL8" s="8"/>
       <c r="AM8" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN8" s="10"/>
       <c r="AO8" s="8"/>
       <c r="AP8" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ8" s="10"/>
       <c r="AR8" s="8"/>
       <c r="AS8" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT8" s="10"/>
       <c r="AU8" s="8"/>
       <c r="AV8" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW8" s="10"/>
       <c r="AX8" s="8"/>
       <c r="AY8" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ8" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA8" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:53" ht="135" x14ac:dyDescent="0.25">
@@ -2812,11 +2856,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2828,6 +2867,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2845,7 +2889,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Avance del diagrama de clases
Avance del diagrama de clases y actualización de plantilla de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 4ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 4ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0BFF09B2-0032-4042-9D56-D593BBCAD538}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630B809A-F8DC-4F3A-8565-66D00D476B13}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="62">
   <si>
     <t>Columna</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>Modulo de pagos, referente al pago de alumno: historial de pago, registro de pago (vista de profesor) incluyedo promociones (CRU). [Desarrollo y pruebas (clases Junit y tablas de pruebas por función)]</t>
+  </si>
+  <si>
+    <t>Hecho</t>
+  </si>
+  <si>
+    <t>En proceso</t>
   </si>
 </sst>
 </file>
@@ -849,10 +855,10 @@
   <dimension ref="B1:BA20"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,7 +1154,7 @@
         <v>40</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="G6" s="5">
         <v>1</v>
@@ -1263,7 +1269,7 @@
         <v>41</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="G7" s="5">
         <v>4</v>
@@ -1390,7 +1396,7 @@
         <v>41</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="G8" s="5">
         <v>2</v>
@@ -1505,7 +1511,7 @@
         <v>40</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="G9" s="5">
         <v>4</v>
@@ -1630,7 +1636,7 @@
         <v>40</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="G10" s="5">
         <v>2</v>
@@ -1862,7 +1868,7 @@
         <v>40</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="G12" s="5">
         <v>1</v>
@@ -1909,60 +1915,62 @@
         <v>1</v>
       </c>
       <c r="AB12" s="10"/>
-      <c r="AC12" s="8"/>
+      <c r="AC12" s="8">
+        <v>3</v>
+      </c>
       <c r="AD12" s="8">
         <f>AA12-AC12</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AE12" s="10"/>
       <c r="AF12" s="8"/>
       <c r="AG12" s="8">
         <f>AD12-AF12</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AH12" s="10"/>
       <c r="AI12" s="8"/>
       <c r="AJ12" s="8">
         <f>AG12-AI12</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AK12" s="10"/>
       <c r="AL12" s="8"/>
       <c r="AM12" s="8">
         <f>AJ12-AL12</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AN12" s="10"/>
       <c r="AO12" s="8"/>
       <c r="AP12" s="8">
         <f>AM12-AO12</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AQ12" s="10"/>
       <c r="AR12" s="8"/>
       <c r="AS12" s="8">
         <f>AP12-AR12</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AT12" s="10"/>
       <c r="AU12" s="8"/>
       <c r="AV12" s="8">
         <f>AS12-AU12</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AW12" s="10"/>
       <c r="AX12" s="8"/>
       <c r="AY12" s="8">
         <f>AV12-AX12</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="AZ12" s="11">
         <f>H12+K12+N12+Q12+T12+W12+Z12+AC12+AF12+AI12+AL12+AO12+AR12+AU12+AX12</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA12" s="11">
         <f>G12-AZ12</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="13" spans="2:53" ht="45" x14ac:dyDescent="0.25">
@@ -2856,6 +2864,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2867,11 +2880,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Diseño del caso de uso Consultar pagos cliente.
Se crea el diagrama de secuencia, robustez y prototipo del caso de uso
consultar pagos cliente.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 4ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 4ta Iteración.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8502A561-8A5F-49E2-86D2-FA99F1A4A132}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="63">
   <si>
     <t>Columna</t>
   </si>
@@ -217,12 +211,15 @@
   </si>
   <si>
     <t>En proceso</t>
+  </si>
+  <si>
+    <t>hecho</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -515,7 +512,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -574,7 +571,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -607,26 +604,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -659,23 +639,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -851,14 +814,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA20"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="AA17" sqref="AA17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2447,7 +2410,7 @@
         <v>41</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="G17" s="5">
         <v>4</v>
@@ -2500,54 +2463,56 @@
         <v>4</v>
       </c>
       <c r="AE17" s="10"/>
-      <c r="AF17" s="8"/>
+      <c r="AF17" s="8">
+        <v>2</v>
+      </c>
       <c r="AG17" s="8">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AH17" s="10"/>
       <c r="AI17" s="8"/>
       <c r="AJ17" s="8">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AK17" s="10"/>
       <c r="AL17" s="8"/>
       <c r="AM17" s="8">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AN17" s="10"/>
       <c r="AO17" s="8"/>
       <c r="AP17" s="8">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AQ17" s="10"/>
       <c r="AR17" s="8"/>
       <c r="AS17" s="8">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AT17" s="10"/>
       <c r="AU17" s="8"/>
       <c r="AV17" s="8">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AW17" s="10"/>
       <c r="AX17" s="8"/>
       <c r="AY17" s="8">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AZ17" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA17" s="11">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:53" x14ac:dyDescent="0.25">
@@ -2866,6 +2831,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2877,11 +2847,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2899,7 +2864,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Integración de paneles de catálogos
Se integran los paneles de catálogos a la ventana principal de director
y pagos de profesor.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 4ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 4ta Iteración.xlsx
@@ -821,7 +821,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AA17" sqref="AA17"/>
+      <selection pane="bottomRight" activeCell="AF15" sqref="AF15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,7 +2063,7 @@
         <v>41</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="G14" s="5">
         <v>3</v>
@@ -2116,54 +2116,56 @@
         <v>3</v>
       </c>
       <c r="AE14" s="10"/>
-      <c r="AF14" s="8"/>
+      <c r="AF14" s="8">
+        <v>1</v>
+      </c>
       <c r="AG14" s="8">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH14" s="10"/>
       <c r="AI14" s="8"/>
       <c r="AJ14" s="8">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AK14" s="10"/>
       <c r="AL14" s="8"/>
       <c r="AM14" s="8">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AN14" s="10"/>
       <c r="AO14" s="8"/>
       <c r="AP14" s="8">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AQ14" s="10"/>
       <c r="AR14" s="8"/>
       <c r="AS14" s="8">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AT14" s="10"/>
       <c r="AU14" s="8"/>
       <c r="AV14" s="8">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AW14" s="10"/>
       <c r="AX14" s="8"/>
       <c r="AY14" s="8">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AZ14" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA14" s="11">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:53" ht="93" customHeight="1" x14ac:dyDescent="0.25">
@@ -2831,11 +2833,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2847,6 +2844,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Reporte de entrega del 40%
Reporte de entrega del 40% y actualización de plantillas de tareas y
casos de uso.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 4ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 4ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7666E59E-B204-4A10-A5F6-B7C1AE0A464E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAFFFD1-BFE4-4A49-BB84-A24FF76C5884}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="61">
   <si>
     <t>Columna</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Mario</t>
   </si>
   <si>
-    <t>Por iniciar</t>
-  </si>
-  <si>
     <t>Desarrollo</t>
   </si>
   <si>
@@ -217,9 +214,6 @@
   </si>
   <si>
     <t>En proceso</t>
-  </si>
-  <si>
-    <t>hecho</t>
   </si>
 </sst>
 </file>
@@ -858,10 +852,10 @@
   <dimension ref="B1:BA20"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AI14" sqref="AI14"/>
+      <selection pane="bottomRight" activeCell="AI15" sqref="AI15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,17 +1141,17 @@
     </row>
     <row r="6" spans="2:53" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>40</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G6" s="5">
         <v>1</v>
@@ -1266,13 +1260,13 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="21" t="s">
         <v>41</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G7" s="5">
         <v>4</v>
@@ -1393,13 +1387,13 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>41</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G8" s="5">
         <v>2</v>
@@ -1508,13 +1502,13 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>40</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G9" s="5">
         <v>4</v>
@@ -1633,13 +1627,13 @@
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G10" s="5">
         <v>2</v>
@@ -1746,17 +1740,17 @@
     </row>
     <row r="11" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="21" t="s">
         <v>41</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="G11" s="5">
         <v>2</v>
@@ -1861,17 +1855,17 @@
     </row>
     <row r="12" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>40</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G12" s="5">
         <v>1</v>
@@ -1980,17 +1974,17 @@
     </row>
     <row r="13" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>41</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="G13" s="5">
         <v>3</v>
@@ -2049,63 +2043,65 @@
         <v>3</v>
       </c>
       <c r="AH13" s="10"/>
-      <c r="AI13" s="8"/>
+      <c r="AI13" s="8">
+        <v>1</v>
+      </c>
       <c r="AJ13" s="8">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AK13" s="10"/>
       <c r="AL13" s="8"/>
       <c r="AM13" s="8">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AN13" s="10"/>
       <c r="AO13" s="8"/>
       <c r="AP13" s="8">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AQ13" s="10"/>
       <c r="AR13" s="8"/>
       <c r="AS13" s="8">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AT13" s="10"/>
       <c r="AU13" s="8"/>
       <c r="AV13" s="8">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AW13" s="10"/>
       <c r="AX13" s="8"/>
       <c r="AY13" s="8">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AZ13" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA13" s="11">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:53" ht="75" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" s="21" t="s">
         <v>41</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G14" s="5">
         <v>3</v>
@@ -2166,63 +2162,65 @@
         <v>2</v>
       </c>
       <c r="AH14" s="10"/>
-      <c r="AI14" s="8"/>
+      <c r="AI14" s="8">
+        <v>2</v>
+      </c>
       <c r="AJ14" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK14" s="10"/>
       <c r="AL14" s="8"/>
       <c r="AM14" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN14" s="10"/>
       <c r="AO14" s="8"/>
       <c r="AP14" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ14" s="10"/>
       <c r="AR14" s="8"/>
       <c r="AS14" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT14" s="10"/>
       <c r="AU14" s="8"/>
       <c r="AV14" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW14" s="10"/>
       <c r="AX14" s="8"/>
       <c r="AY14" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ14" s="11">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BA14" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:53" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G15" s="5">
         <v>3</v>
@@ -2329,17 +2327,17 @@
     </row>
     <row r="16" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>40</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="G16" s="5">
         <v>2</v>
@@ -2398,63 +2396,65 @@
         <v>2</v>
       </c>
       <c r="AH16" s="10"/>
-      <c r="AI16" s="8"/>
+      <c r="AI16" s="8">
+        <v>3</v>
+      </c>
       <c r="AJ16" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AK16" s="10"/>
       <c r="AL16" s="8"/>
       <c r="AM16" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AN16" s="10"/>
       <c r="AO16" s="8"/>
       <c r="AP16" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AQ16" s="10"/>
       <c r="AR16" s="8"/>
       <c r="AS16" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AT16" s="10"/>
       <c r="AU16" s="8"/>
       <c r="AV16" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AW16" s="10"/>
       <c r="AX16" s="8"/>
       <c r="AY16" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="AZ16" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA16" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="17" spans="2:53" ht="90" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G17" s="5">
         <v>4</v>
@@ -2875,11 +2875,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2891,6 +2886,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>